<commit_message>
added macy.js layout and fixes
</commit_message>
<xml_diff>
--- a/GradedExercise - Copy.xlsx
+++ b/GradedExercise - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HS19_projects\webeC\hs19-cr-webec-ge-lucafluri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497B7D6D-C5E1-44D4-BE79-DB62DB8F5ADD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF38F02-3DF2-46B9-BF10-391DCD89206F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:E18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -724,14 +724,14 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D4" s="14">
-        <v>5</v>
-      </c>
-      <c r="E4" s="14" t="s">
+      <c r="D4" s="13">
+        <v>5</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>6</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
@@ -761,11 +761,11 @@
       </c>
       <c r="G6" s="3">
         <f>SUM(G4:G5)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H6" s="3">
         <f>MIN(C6,G6)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
@@ -776,7 +776,7 @@
         <v>2</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -787,18 +787,18 @@
         <v>3</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>3</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -820,7 +820,7 @@
         <v>7</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
@@ -850,11 +850,11 @@
       </c>
       <c r="G14" s="3">
         <f>SUM(G8:G13)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H14" s="3">
         <f>MIN(C14,G14)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
@@ -869,7 +869,7 @@
         <v>10</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -880,7 +880,7 @@
         <v>13</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -891,7 +891,7 @@
         <v>12</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>11</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -954,11 +954,11 @@
       </c>
       <c r="G23" s="3">
         <f>SUM(G16:G22)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H23" s="3">
         <f>MIN(C23,G23)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
         <v>22</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1032,11 +1032,11 @@
       </c>
       <c r="G30" s="3">
         <f>SUM(G25:G29)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H30" s="3">
         <f>MIN(C30,G30)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="10">
         <f>SUM(H4:H30)</f>
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
       <c r="H40" s="9"/>
       <c r="I40" s="9">
         <f>Bonus-Malus</f>
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
       <c r="H42" s="4"/>
       <c r="I42" s="5">
         <f>1 + TOTAL/10</f>
-        <v>1</v>
+        <v>5.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added index page controller
</commit_message>
<xml_diff>
--- a/GradedExercise - Copy.xlsx
+++ b/GradedExercise - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HS19_projects\webeC\hs19-cr-webec-ge-lucafluri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D05D24-1E86-4910-9356-2936A66B1416}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0872D8DF-AC34-4BD6-BEAD-73296F013F56}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>It works</t>
   </si>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -906,14 +906,14 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="14">
+        <v>2</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -954,11 +954,11 @@
       </c>
       <c r="G23" s="3">
         <f>SUM(G16:G22)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H23" s="3">
         <f>MIN(C23,G23)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="10">
         <f>SUM(H4:H30)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
       <c r="H40" s="9"/>
       <c r="I40" s="9">
         <f>Bonus-Malus</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
       <c r="H42" s="4"/>
       <c r="I42" s="5">
         <f>1 + TOTAL/10</f>
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed picture to favorite
</commit_message>
<xml_diff>
--- a/GradedExercise - Copy.xlsx
+++ b/GradedExercise - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HS19_projects\webeC\hs19-cr-webec-ge-lucafluri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6899CC82-9EE1-4181-85DE-C148DD858620}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B86D74-9143-40CA-9B05-CE9679A055E4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>It works</t>
   </si>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -873,10 +873,10 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D17" s="14">
-        <v>5</v>
-      </c>
-      <c r="E17" s="14" t="s">
+      <c r="D17" s="13">
+        <v>5</v>
+      </c>
+      <c r="E17" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G17">
@@ -884,10 +884,10 @@
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" s="14">
-        <v>2</v>
-      </c>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="13">
+        <v>2</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G18">

</xml_diff>